<commit_message>
terceiro dual simplex finalizado
</commit_message>
<xml_diff>
--- a/simplex_revisado.xlsx
+++ b/simplex_revisado.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acsjunior/Documents/Projects/ppgmne-mnum7078/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC55E31-CD78-F74D-99F4-81378CC952C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39251222-F9C1-6944-A86B-DA98662D8D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{EAF9DF70-EF61-6647-8354-71546881E2E1}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="2" xr2:uid="{EAF9DF70-EF61-6647-8354-71546881E2E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Simplex" sheetId="1" r:id="rId1"/>
     <sheet name="Simplex revisado" sheetId="3" r:id="rId2"/>
+    <sheet name="dualidade" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="73">
   <si>
     <t>Max z = 3x1 + 4x2</t>
   </si>
@@ -206,6 +207,45 @@
   </si>
   <si>
     <t>1x1 + 2x2 &gt;= 4</t>
+  </si>
+  <si>
+    <t>Primal</t>
+  </si>
+  <si>
+    <t>sa:</t>
+  </si>
+  <si>
+    <t>Ax &lt;= b</t>
+  </si>
+  <si>
+    <t>x &gt;= 0</t>
+  </si>
+  <si>
+    <t>Dual</t>
+  </si>
+  <si>
+    <t>y &gt;= 0</t>
+  </si>
+  <si>
+    <t>Min w = b^t*y</t>
+  </si>
+  <si>
+    <t>Max z = c^t*x</t>
+  </si>
+  <si>
+    <t>yA &gt;= c (ou A^t*y &gt;= c)</t>
+  </si>
+  <si>
+    <t>Min z = c^t*x</t>
+  </si>
+  <si>
+    <t>Ax &gt;= b</t>
+  </si>
+  <si>
+    <t>Max w = b^t*y</t>
+  </si>
+  <si>
+    <t>yA &lt;= c</t>
   </si>
 </sst>
 </file>
@@ -969,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0E0CC4-01A9-D14C-9388-46A784C5AEB8}">
   <dimension ref="A1:P119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -4174,8 +4214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E01435-9D0E-2B44-A85C-07D10F261D9D}">
   <dimension ref="A1:O130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E130" sqref="E130"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6687,4 +6727,95 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15843148-2834-7441-B1EF-A747070EAE0D}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>